<commit_message>
Generation of instances similar to Templemeier 1996
</commit_message>
<xml_diff>
--- a/Instances/01_NonStationary.xlsx
+++ b/Instances/01_NonStationary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -46,7 +46,10 @@
     <t>NonStationary</t>
   </si>
   <si>
-    <t>NrTimeBucketWithoutUncertainty</t>
+    <t>NrTimeBucketWithoutUncertaintyBefore</t>
+  </si>
+  <si>
+    <t>NrTimeBucketWithoutUncertaintyAfter</t>
   </si>
   <si>
     <t>Manuf_0001</t>
@@ -443,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,7 +488,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -509,6 +512,14 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
         <v>3</v>
       </c>
     </row>
@@ -533,33 +544,33 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -588,7 +599,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -617,7 +628,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -646,7 +657,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -675,7 +686,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -704,7 +715,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -733,7 +744,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -762,7 +773,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -810,33 +821,33 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -848,7 +859,7 @@
         <v>0.026</v>
       </c>
       <c r="E2" t="n">
-        <v>2.754375</v>
+        <v>9.500400000000001</v>
       </c>
       <c r="F2" t="n">
         <v>0.26</v>
@@ -865,7 +876,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -877,7 +888,7 @@
         <v>0.0248</v>
       </c>
       <c r="E3" t="n">
-        <v>1.10515</v>
+        <v>3.4752</v>
       </c>
       <c r="F3" t="n">
         <v>0.248</v>
@@ -894,19 +905,19 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>828</v>
+        <v>895</v>
       </c>
       <c r="D4" t="n">
         <v>0.0048</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7224000000000002</v>
+        <v>4.0816</v>
       </c>
       <c r="F4" t="n">
         <v>0.048</v>
@@ -923,19 +934,19 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>828</v>
+        <v>895</v>
       </c>
       <c r="D5" t="n">
         <v>0.002</v>
       </c>
       <c r="E5" t="n">
-        <v>0.301</v>
+        <v>1.700666666666667</v>
       </c>
       <c r="F5" t="n">
         <v>0.02</v>
@@ -952,19 +963,19 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="n">
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>828</v>
+        <v>895</v>
       </c>
       <c r="D6" t="n">
         <v>0.0036</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5418000000000001</v>
+        <v>3.0612</v>
       </c>
       <c r="F6" t="n">
         <v>0.036</v>
@@ -981,19 +992,19 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>445</v>
+        <v>522</v>
       </c>
       <c r="D7" t="n">
         <v>0.026</v>
       </c>
       <c r="E7" t="n">
-        <v>2.328625</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
         <v>0.26</v>
@@ -1010,7 +1021,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -1022,7 +1033,7 @@
         <v>0.0508</v>
       </c>
       <c r="E8" t="n">
-        <v>0.83185</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
         <v>0.508</v>
@@ -1039,19 +1050,19 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D9" t="n">
         <v>0.0248</v>
       </c>
       <c r="E9" t="n">
-        <v>0.6990500000000002</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
         <v>0.248</v>
@@ -1087,28 +1098,28 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1131,13 +1142,13 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="H2" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I2" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1160,13 +1171,13 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>197</v>
+        <v>246</v>
       </c>
       <c r="H3" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I3" t="n">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1189,13 +1200,13 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>261</v>
+        <v>287</v>
       </c>
       <c r="H4" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I4" t="n">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1218,13 +1229,13 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>220</v>
+        <v>259</v>
       </c>
       <c r="H5" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I5" t="n">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1247,13 +1258,13 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>220</v>
+        <v>268</v>
       </c>
       <c r="H6" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I6" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1276,13 +1287,13 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>290</v>
+        <v>227</v>
       </c>
       <c r="H7" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I7" t="n">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1306,28 +1317,28 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1350,13 +1361,13 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>6.124999999999998</v>
+        <v>6.799999999999999</v>
       </c>
       <c r="H2" t="n">
-        <v>1.1</v>
+        <v>1.075</v>
       </c>
       <c r="I2" t="n">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1379,13 +1390,13 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>9.357499999999998</v>
+        <v>11.685</v>
       </c>
       <c r="H3" t="n">
-        <v>2.089999999999999</v>
+        <v>2.137499999999999</v>
       </c>
       <c r="I3" t="n">
-        <v>3.419999999999999</v>
+        <v>3.562499999999999</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1408,13 +1419,13 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>17.68275</v>
+        <v>19.44424999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>2.980999999999999</v>
+        <v>3.184249999999999</v>
       </c>
       <c r="I4" t="n">
-        <v>5.352249999999998</v>
+        <v>5.013499999999999</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1437,13 +1448,13 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>18.9145</v>
+        <v>22.267525</v>
       </c>
       <c r="H5" t="n">
-        <v>3.696925</v>
+        <v>3.7829</v>
       </c>
       <c r="I5" t="n">
-        <v>6.792025</v>
+        <v>6.5341</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1466,13 +1477,13 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>22.52305</v>
+        <v>27.43716999999999</v>
       </c>
       <c r="H6" t="n">
-        <v>4.606987499999999</v>
+        <v>4.709364999999999</v>
       </c>
       <c r="I6" t="n">
-        <v>7.883067499999998</v>
+        <v>7.985444999999999</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1495,13 +1506,13 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>33.9705275</v>
+        <v>26.59072325</v>
       </c>
       <c r="H7" t="n">
-        <v>4.919869499999999</v>
+        <v>5.03700925</v>
       </c>
       <c r="I7" t="n">
-        <v>8.434061999999999</v>
+        <v>9.254040249999999</v>
       </c>
     </row>
   </sheetData>
@@ -1515,7 +1526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1533,7 +1544,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>11300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1541,7 +1552,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>3565</v>
+        <v>8503.333333333332</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1549,47 +1560,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>4013.333333333334</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>8026.666666666668</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>20066.66666666667</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>4776.666666666667</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>436.6666666666666</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>751.6666666666667</v>
+        <v>45067.66666666666</v>
       </c>
     </row>
   </sheetData>
@@ -1603,7 +1574,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1611,7 +1582,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
@@ -1621,83 +1592,38 @@
       <c r="D1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
         <v>10</v>
       </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>3</v>
-      </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -1706,27 +1632,12 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -1735,27 +1646,12 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -1764,27 +1660,12 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>5</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -1795,25 +1676,10 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>2</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -1824,25 +1690,10 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -1852,21 +1703,6 @@
       </c>
       <c r="D9" t="n">
         <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>